<commit_message>
add GV main layout
</commit_message>
<xml_diff>
--- a/server/giangViens - Copy.xlsx
+++ b/server/giangViens - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\QuanLyKhoaLuan\quan-ly-khoa-luan\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12D9F5-3E63-44DF-81FD-96BB2A229DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D5A55B-C687-497C-B8A7-4AF901FEFB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3336" yWindow="1872" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,16 +51,16 @@
     <t>AI</t>
   </si>
   <si>
-    <t>Giang vien moi</t>
-  </si>
-  <si>
-    <t>0800000111</t>
-  </si>
-  <si>
-    <t>gvm@uit.edu.vn</t>
-  </si>
-  <si>
-    <t>111</t>
+    <t>GV Thịnh Nguyễn</t>
+  </si>
+  <si>
+    <t>0383965078</t>
+  </si>
+  <si>
+    <t>thinhndp13@uit.edu.vn</t>
+  </si>
+  <si>
+    <t>1313</t>
   </si>
 </sst>
 </file>

</xml_diff>